<commit_message>
Update Auth Server Form Validation
</commit_message>
<xml_diff>
--- a/excel_templates/sample_workbook.xlsx
+++ b/excel_templates/sample_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewh\Dropbox\Gav\My Documents\Juniper Scripts\junos-config-templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE1B5DD-9E32-4920-9A76-0BD9FE96DB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC56D7-613B-45EF-B333-2DB85710AAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="2055" windowWidth="32385" windowHeight="18060" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
+    <workbookView xWindow="23820" yWindow="5730" windowWidth="22485" windowHeight="14355" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{1C2DD157-0169-4B11-8524-207EA96CC6F9}">
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{1C2DD157-0169-4B11-8524-207EA96CC6F9}">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="854">
   <si>
     <t>Name</t>
   </si>
@@ -2656,6 +2656,18 @@
   </si>
   <si>
     <t>RADIUS</t>
+  </si>
+  <si>
+    <t>Authentication Server Key</t>
+  </si>
+  <si>
+    <t>Super-User</t>
+  </si>
+  <si>
+    <t>key1234</t>
+  </si>
+  <si>
+    <t>192.168.1.13</t>
   </si>
 </sst>
 </file>
@@ -3533,6 +3545,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3614,16 +3629,25 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3886,8 +3910,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FEC8904D-0887-4DC9-91F8-F0E825A65E78}" name="Table4" displayName="Table4" ref="A1:D19" totalsRowShown="0">
   <autoFilter ref="A1:D19" xr:uid="{FEC8904D-0887-4DC9-91F8-F0E825A65E78}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{02D56E0C-A9AB-48E1-AFFA-E5E02F3E2F12}" name="Name" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{F9C08807-8C12-428F-A32D-180C2802D056}" name="Screen" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{02D56E0C-A9AB-48E1-AFFA-E5E02F3E2F12}" name="Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F9C08807-8C12-428F-A32D-180C2802D056}" name="Screen" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{19B0833B-4285-431D-822B-48892AE9BD76}" name="Services"/>
     <tableColumn id="4" xr3:uid="{41D75EC5-B677-43F1-A178-BBEB818715B6}" name="vrf"/>
   </tableColumns>
@@ -3900,7 +3924,7 @@
   <autoFilter ref="A1:H44" xr:uid="{5E4FD355-8A3A-4575-B8B9-2033F405DE5A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EAF6C448-8196-46EC-B0A8-9AD31A19C745}" name="Interface"/>
-    <tableColumn id="2" xr3:uid="{92059489-9031-489B-9C37-4FCAF69EDF76}" name="Logical Unit" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{92059489-9031-489B-9C37-4FCAF69EDF76}" name="Logical Unit" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{00BAE52F-18DA-4137-A0FC-561859E617DC}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FCD0FFF9-2473-403E-A22A-89493E29FB8E}" name="Type"/>
     <tableColumn id="5" xr3:uid="{0482F9E2-925C-434A-853B-05259A65B30F}" name="Family"/>
@@ -3939,7 +3963,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}" name="Table7" displayName="Table7" ref="A1:M200" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}" name="Table7" displayName="Table7" ref="A1:M200" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:M200" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C547259A-7983-45F7-895E-1EFC74765110}" name="From Zone"/>
@@ -3961,7 +3985,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FDCF5AD-E100-4012-9806-A624A022335C}" name="Table73" displayName="Table73" ref="A1:I200" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FDCF5AD-E100-4012-9806-A624A022335C}" name="Table73" displayName="Table73" ref="A1:I200" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:I200" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}"/>
   <tableColumns count="9">
     <tableColumn id="14" xr3:uid="{6C4F03B8-D3CF-4725-AB73-216B28241D58}" name="Type"/>
@@ -4295,10 +4319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68590D1-FAE6-4DDC-BE52-A7BC10F9195F}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4313,7 +4337,7 @@
         <v>279</v>
       </c>
       <c r="B1" s="58"/>
-      <c r="C1" s="87"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -4322,7 +4346,7 @@
       <c r="B2" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="C2" s="87"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4331,7 +4355,7 @@
       <c r="B3" s="7" t="s">
         <v>807</v>
       </c>
-      <c r="C3" s="87"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="4" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -4546,101 +4570,115 @@
       <c r="A28" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>851</v>
+      </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>659</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="7" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>660</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7">
+        <v>1812</v>
+      </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="58" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>850</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="58" t="s">
         <v>650</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>638</v>
-      </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="58"/>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>13</v>
+        <v>641</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>647</v>
+        <v>13</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>651</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B43" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="5"/>
+      <c r="C43" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4648,39 +4686,49 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="C1:C3"/>
   </mergeCells>
   <conditionalFormatting sqref="A28:A30">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$B$27="Local Password Only"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B7 B10:B13 B16:B19">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"CUSTOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B30">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>AND(B28="",NOT($B$27="Local Password Only"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C13">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($C10="",OR($B$13="Primary",$B$13="Secondary"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <conditionalFormatting sqref="A31">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B$27="Local Password Only"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(B31="",NOT($B$27="Local Password Only"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:C13" xr:uid="{BBB311CD-DCE0-4F50-8AA7-192F74EA4323}">
       <formula1>"Primary,Secondary,Standalone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B42 B29:B30" xr:uid="{630055D3-5F05-4459-B277-484F4CDA34FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:B43" xr:uid="{630055D3-5F05-4459-B277-484F4CDA34FD}">
       <formula1>"Enabled"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27" xr:uid="{9195BDEB-943C-4F04-8A7A-DDEC02878F23}">
@@ -4689,6 +4737,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28" xr:uid="{D57F6CA5-45D7-4BE1-9FEF-6ADCE826F555}">
       <formula1>"Super-User,Operator,Read-Only,Unauthorized,CUSTOM"</formula1>
     </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30" xr:uid="{01D6448D-D68A-42E1-B29E-3074EE373FD6}">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31" xr:uid="{6965DBEE-CECB-42BF-B53A-0F6F4BAE6BC2}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{AC6D60F8-44CB-4868-9431-53A6D678CD1D}"/>
@@ -6883,15 +6935,15 @@
       </c>
       <c r="U2" s="3" t="str">
         <f>IF(ISBLANK(System!$B$28),"",System!$B$28)</f>
-        <v/>
-      </c>
-      <c r="V2" s="3" t="str">
-        <f>IF(ISBLANK(System!$B$29),"",System!$B$29)</f>
-        <v/>
-      </c>
-      <c r="W2" s="3" t="str">
+        <v>Super-User</v>
+      </c>
+      <c r="V2" s="3" t="e">
+        <f>IF(ISBLANK(System!#REF!),"",System!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="W2" s="3">
         <f>IF(ISBLANK(System!$B$30),"",System!$B$30)</f>
-        <v/>
+        <v>1812</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7053,27 +7105,27 @@
       <c r="A24" s="56"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="str">
-        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$29),"",System!$B$29))</f>
-        <v/>
+      <c r="A25" s="56" t="e">
+        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!#REF!),"",System!#REF!))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="str">
+      <c r="A26" s="56">
         <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$30),"",System!$B$30))</f>
-        <v/>
+        <v>1812</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="str">
-        <f>IF(ISBLANK(System!$B$29),"",System!$B$29)</f>
-        <v/>
+      <c r="A27" s="56" t="e">
+        <f>IF(ISBLANK(System!#REF!),"",System!#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="str">
+      <c r="A28" s="56">
         <f>IF(ISBLANK(System!$B$30),"",System!$B$30)</f>
-        <v/>
+        <v>1812</v>
       </c>
     </row>
   </sheetData>
@@ -12361,7 +12413,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>714</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -12371,42 +12423,42 @@
         <f ca="1">MID(CELL("filename",D1),FIND("]",CELL("filename",D1))+1,11)</f>
         <v>srx1600-phy</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="66" t="s">
         <v>664</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="68"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
+      <c r="A2" s="64"/>
       <c r="B2" s="13" t="s">
         <v>665</v>
       </c>
       <c r="C2" s="15"/>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="66" t="s">
         <v>666</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="68"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="13" t="s">
         <v>667</v>
       </c>
@@ -12444,50 +12496,50 @@
       <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="64"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="13" t="s">
         <v>675</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>676</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="69" t="s">
         <v>664</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="71"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="63" t="s">
         <v>715</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="72" t="s">
         <v>677</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="79" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="80" t="s">
         <v>678</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
       <c r="J5" s="24" t="s">
         <v>679</v>
       </c>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="83" t="s">
         <v>680</v>
       </c>
-      <c r="L5" s="83"/>
+      <c r="L5" s="84"/>
       <c r="M5" s="25" t="s">
         <v>681</v>
       </c>
@@ -12496,24 +12548,24 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="84" t="s">
+      <c r="A6" s="64"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="85" t="s">
         <v>683</v>
       </c>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
       <c r="J6" s="26" t="s">
         <v>684</v>
       </c>
-      <c r="K6" s="60" t="s">
+      <c r="K6" s="61" t="s">
         <v>685</v>
       </c>
-      <c r="L6" s="61"/>
+      <c r="L6" s="62"/>
       <c r="M6" s="27" t="s">
         <v>686</v>
       </c>
@@ -12522,9 +12574,9 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="77"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="78"/>
       <c r="D7" s="28" t="s">
         <v>688</v>
       </c>
@@ -12560,9 +12612,9 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="78"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="35" t="s">
         <v>696</v>
       </c>

</xml_diff>

<commit_message>
Update Auth Server Values in xlt
</commit_message>
<xml_diff>
--- a/excel_templates/sample_workbook.xlsx
+++ b/excel_templates/sample_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewh\Dropbox\Gav\My Documents\Juniper Scripts\junos-config-templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC56D7-613B-45EF-B333-2DB85710AAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF58464A-2076-4391-9068-EF1035F641C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23820" yWindow="5730" windowWidth="22485" windowHeight="14355" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="71640" windowHeight="21120" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -2655,9 +2655,6 @@
     <t>junos-winframe</t>
   </si>
   <si>
-    <t>RADIUS</t>
-  </si>
-  <si>
     <t>Authentication Server Key</t>
   </si>
   <si>
@@ -2668,6 +2665,9 @@
   </si>
   <si>
     <t>192.168.1.13</t>
+  </si>
+  <si>
+    <t>Local Password Only</t>
   </si>
 </sst>
 </file>
@@ -3414,7 +3414,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3629,25 +3629,16 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -3910,8 +3901,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FEC8904D-0887-4DC9-91F8-F0E825A65E78}" name="Table4" displayName="Table4" ref="A1:D19" totalsRowShown="0">
   <autoFilter ref="A1:D19" xr:uid="{FEC8904D-0887-4DC9-91F8-F0E825A65E78}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{02D56E0C-A9AB-48E1-AFFA-E5E02F3E2F12}" name="Name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{F9C08807-8C12-428F-A32D-180C2802D056}" name="Screen" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{02D56E0C-A9AB-48E1-AFFA-E5E02F3E2F12}" name="Name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{F9C08807-8C12-428F-A32D-180C2802D056}" name="Screen" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{19B0833B-4285-431D-822B-48892AE9BD76}" name="Services"/>
     <tableColumn id="4" xr3:uid="{41D75EC5-B677-43F1-A178-BBEB818715B6}" name="vrf"/>
   </tableColumns>
@@ -3924,7 +3915,7 @@
   <autoFilter ref="A1:H44" xr:uid="{5E4FD355-8A3A-4575-B8B9-2033F405DE5A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EAF6C448-8196-46EC-B0A8-9AD31A19C745}" name="Interface"/>
-    <tableColumn id="2" xr3:uid="{92059489-9031-489B-9C37-4FCAF69EDF76}" name="Logical Unit" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{92059489-9031-489B-9C37-4FCAF69EDF76}" name="Logical Unit" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{00BAE52F-18DA-4137-A0FC-561859E617DC}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FCD0FFF9-2473-403E-A22A-89493E29FB8E}" name="Type"/>
     <tableColumn id="5" xr3:uid="{0482F9E2-925C-434A-853B-05259A65B30F}" name="Family"/>
@@ -3963,7 +3954,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}" name="Table7" displayName="Table7" ref="A1:M200" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}" name="Table7" displayName="Table7" ref="A1:M200" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:M200" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C547259A-7983-45F7-895E-1EFC74765110}" name="From Zone"/>
@@ -3985,7 +3976,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FDCF5AD-E100-4012-9806-A624A022335C}" name="Table73" displayName="Table73" ref="A1:I200" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FDCF5AD-E100-4012-9806-A624A022335C}" name="Table73" displayName="Table73" ref="A1:I200" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:I200" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}"/>
   <tableColumns count="9">
     <tableColumn id="14" xr3:uid="{6C4F03B8-D3CF-4725-AB73-216B28241D58}" name="Type"/>
@@ -4322,7 +4313,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4562,7 +4553,7 @@
         <v>658</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -4571,7 +4562,7 @@
         <v>661</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -4580,24 +4571,24 @@
         <v>659</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>660</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="88">
         <v>1812</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C31" s="5"/>
     </row>
@@ -4689,39 +4680,29 @@
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="C1:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A28:A30">
-    <cfRule type="expression" dxfId="6" priority="5">
+  <conditionalFormatting sqref="A28:A31">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$B$27="Local Password Only"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B7 B10:B13 B16:B19">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"CUSTOM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:B30">
-    <cfRule type="expression" dxfId="3" priority="7">
+  <conditionalFormatting sqref="B28:B31">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(B28="",NOT($B$27="Local Password Only"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND($C10="",OR($B$13="Primary",$B$13="Secondary"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B$27="Local Password Only"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(B31="",NOT($B$27="Local Password Only"))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -4768,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B0E9E4-2C99-447E-AD7F-0A18AC94CE6D}">
   <dimension ref="A1:E350"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6745,20 +6726,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D16D872-2573-45BF-9287-60998C8758FD}">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="22" width="15.140625" customWidth="1"/>
+    <col min="9" max="19" width="15.140625" customWidth="1"/>
+    <col min="20" max="20" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>System!A2</f>
         <v>Company Name</v>
@@ -6851,8 +6837,12 @@
         <f>System!A30</f>
         <v>Authentication Server Port</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="str">
+        <f>System!A31</f>
+        <v>Authentication Server Key</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK(System!$B$2),"",System!$B$2)</f>
         <v>BrightNet</v>
@@ -6931,22 +6921,26 @@
       </c>
       <c r="T2" s="3" t="str">
         <f>IF(ISBLANK(System!$B$27),"",System!$B$27)</f>
-        <v>RADIUS</v>
+        <v>Local Password Only</v>
       </c>
       <c r="U2" s="3" t="str">
         <f>IF(ISBLANK(System!$B$28),"",System!$B$28)</f>
         <v>Super-User</v>
       </c>
-      <c r="V2" s="3" t="e">
-        <f>IF(ISBLANK(System!#REF!),"",System!#REF!)</f>
-        <v>#REF!</v>
+      <c r="V2" s="3" t="str">
+        <f>IF(ISBLANK(System!$B$29),"",System!$B$29)</f>
+        <v>192.168.1.13</v>
       </c>
       <c r="W2" s="3">
         <f>IF(ISBLANK(System!$B$30),"",System!$B$30)</f>
         <v>1812</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="3" t="str">
+        <f>IF(ISBLANK(System!$B$31),"",System!$B$31)</f>
+        <v>key1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$2),"",System!$B$2))</f>
         <v>BrightNet</v>
@@ -7025,53 +7019,69 @@
       </c>
       <c r="T3" s="3" t="str">
         <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$27),"",System!$B$27))</f>
-        <v>RADIUS</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+        <v>Local Password Only</v>
+      </c>
+      <c r="U3" s="3" t="str">
+        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$28),"",System!$B$28))</f>
+        <v>Super-User</v>
+      </c>
+      <c r="V3" s="3" t="str">
+        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$29),"",System!$B$29))</f>
+        <v>192.168.1.13</v>
+      </c>
+      <c r="W3" s="3">
+        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$30),"",System!$B$30))</f>
+        <v>1812</v>
+      </c>
+      <c r="X3" s="3" t="str">
+        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$31),"",System!$B$31))</f>
+        <v>key1234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G5" s="56"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="56"/>
       <c r="G6" s="56"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="56"/>
       <c r="G7" s="56"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="56"/>
       <c r="G8" s="56"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="56"/>
       <c r="G9" s="56"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
       <c r="G10" s="56"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="G11" s="56"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
       <c r="G12" s="56"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
       <c r="G13" s="56"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="56"/>
       <c r="G14" s="56"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="56"/>
       <c r="G15" s="56"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="56"/>
       <c r="G16" s="56"/>
     </row>
@@ -7139,7 +7149,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resolve excel formula bug
</commit_message>
<xml_diff>
--- a/excel_templates/sample_workbook.xlsx
+++ b/excel_templates/sample_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewh\Dropbox\Gav\My Documents\Juniper Scripts\junos-config-templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF58464A-2076-4391-9068-EF1035F641C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06466E68-67D5-49C6-BFEC-0FB08BD0C8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="71640" windowHeight="21120" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
+    <workbookView xWindow="18090" yWindow="930" windowWidth="22485" windowHeight="14355" activeTab="2" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -3539,6 +3539,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3628,9 +3631,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4312,7 +4312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68590D1-FAE6-4DDC-BE52-A7BC10F9195F}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -4324,11 +4324,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -4337,7 +4337,7 @@
       <c r="B2" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="C2" s="60"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4346,7 +4346,7 @@
       <c r="B3" s="7" t="s">
         <v>807</v>
       </c>
-      <c r="C3" s="60"/>
+      <c r="C3" s="61"/>
     </row>
     <row r="4" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -4393,11 +4393,11 @@
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="60" t="s">
         <v>653</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -4449,10 +4449,10 @@
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4542,10 +4542,10 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="59" t="s">
         <v>657</v>
       </c>
-      <c r="B26" s="58"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4578,7 +4578,7 @@
       <c r="A30" s="6" t="s">
         <v>660</v>
       </c>
-      <c r="B30" s="88">
+      <c r="B30" s="58">
         <v>1812</v>
       </c>
       <c r="C30" s="5"/>
@@ -4593,10 +4593,10 @@
       <c r="C31" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="58" t="s">
+      <c r="A33" s="59" t="s">
         <v>650</v>
       </c>
-      <c r="B33" s="58"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6729,7 +6729,7 @@
   <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,28 +7115,16 @@
       <c r="A24" s="56"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="e">
-        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!#REF!),"",System!#REF!))</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A25" s="56"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56">
-        <f>IF(ISBLANK(System!$C$10),"",IF(ISBLANK(System!$B$30),"",System!$B$30))</f>
-        <v>1812</v>
-      </c>
+      <c r="A26" s="56"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="e">
-        <f>IF(ISBLANK(System!#REF!),"",System!#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A27" s="56"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56">
-        <f>IF(ISBLANK(System!$B$30),"",System!$B$30)</f>
-        <v>1812</v>
-      </c>
+      <c r="A28" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7148,7 +7136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B921653-A31E-4A4F-AA14-15BAA78797BE}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -12423,7 +12411,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>714</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -12433,42 +12421,42 @@
         <f ca="1">MID(CELL("filename",D1),FIND("]",CELL("filename",D1))+1,11)</f>
         <v>srx1600-phy</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="67" t="s">
         <v>664</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="69"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
+      <c r="A2" s="65"/>
       <c r="B2" s="13" t="s">
         <v>665</v>
       </c>
       <c r="C2" s="15"/>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="67" t="s">
         <v>666</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="69"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
+      <c r="A3" s="65"/>
       <c r="B3" s="13" t="s">
         <v>667</v>
       </c>
@@ -12506,50 +12494,50 @@
       <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="13" t="s">
         <v>675</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>676</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="70" t="s">
         <v>664</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="72"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="64" t="s">
         <v>715</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="73" t="s">
         <v>677</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="80" t="s">
+      <c r="C5" s="77"/>
+      <c r="D5" s="81" t="s">
         <v>678</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
       <c r="J5" s="24" t="s">
         <v>679</v>
       </c>
-      <c r="K5" s="83" t="s">
+      <c r="K5" s="84" t="s">
         <v>680</v>
       </c>
-      <c r="L5" s="84"/>
+      <c r="L5" s="85"/>
       <c r="M5" s="25" t="s">
         <v>681</v>
       </c>
@@ -12558,24 +12546,24 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="85" t="s">
+      <c r="A6" s="65"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="86" t="s">
         <v>683</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
       <c r="J6" s="26" t="s">
         <v>684</v>
       </c>
-      <c r="K6" s="61" t="s">
+      <c r="K6" s="62" t="s">
         <v>685</v>
       </c>
-      <c r="L6" s="62"/>
+      <c r="L6" s="63"/>
       <c r="M6" s="27" t="s">
         <v>686</v>
       </c>
@@ -12584,9 +12572,9 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="78"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="28" t="s">
         <v>688</v>
       </c>
@@ -12622,9 +12610,9 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="79"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="35" t="s">
         <v>696</v>
       </c>

</xml_diff>

<commit_message>
Correct Inferface map in excel template
</commit_message>
<xml_diff>
--- a/excel_templates/sample_workbook.xlsx
+++ b/excel_templates/sample_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewh\Dropbox\Gav\My Documents\Juniper Scripts\junos-config-templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06466E68-67D5-49C6-BFEC-0FB08BD0C8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57B5508-DB2A-4B6C-9EC6-7BF1C3DF5B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18090" yWindow="930" windowWidth="22485" windowHeight="14355" activeTab="2" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
+    <workbookView xWindow="37950" yWindow="0" windowWidth="38610" windowHeight="20880" activeTab="8" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="860">
   <si>
     <t>Name</t>
   </si>
@@ -2248,426 +2248,444 @@
     <t>100G Available</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>memberOf</t>
+  </si>
+  <si>
+    <t>vrf</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>BrightNet</t>
+  </si>
+  <si>
+    <t>Gavin White</t>
+  </si>
+  <si>
+    <t>PO Box 143, Upper Coomera QLD 4209</t>
+  </si>
+  <si>
+    <t>1300 024 677</t>
+  </si>
+  <si>
+    <t>support@brightnet.com.au</t>
+  </si>
+  <si>
+    <t>SRX345</t>
+  </si>
+  <si>
+    <t>SD586932XT</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>PBK_RTR2</t>
+  </si>
+  <si>
+    <t>SD586955PN</t>
+  </si>
+  <si>
+    <t>brightnet.com.au</t>
+  </si>
+  <si>
+    <t>1.1.1.1, 8.8.8.8</t>
+  </si>
+  <si>
+    <t>4.4.4.4</t>
+  </si>
+  <si>
+    <t>192.168.1.12</t>
+  </si>
+  <si>
+    <t>paperbark</t>
+  </si>
+  <si>
+    <t>192.168.1.11</t>
+  </si>
+  <si>
+    <t>192.168.1.10</t>
+  </si>
+  <si>
+    <t>ike</t>
+  </si>
+  <si>
+    <t>dmz</t>
+  </si>
+  <si>
+    <t>mgmt</t>
+  </si>
+  <si>
+    <t>ssh, ping</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>ping</t>
+  </si>
+  <si>
+    <t>ge-0/0/1</t>
+  </si>
+  <si>
+    <t>ge-0/0/2</t>
+  </si>
+  <si>
+    <t>ge-0/0/4</t>
+  </si>
+  <si>
+    <t>DMZ Interface</t>
+  </si>
+  <si>
+    <t>Management Interface</t>
+  </si>
+  <si>
+    <t>Guest Network</t>
+  </si>
+  <si>
+    <t>Internal Network</t>
+  </si>
+  <si>
+    <t>192.168.100.1/24</t>
+  </si>
+  <si>
+    <t>192.168.10.1/24</t>
+  </si>
+  <si>
+    <t>192.168.1.1/24</t>
+  </si>
+  <si>
+    <t>192.168.99.1/24</t>
+  </si>
+  <si>
+    <t>net_mgmt</t>
+  </si>
+  <si>
+    <t>net_guest</t>
+  </si>
+  <si>
+    <t>net_internal</t>
+  </si>
+  <si>
+    <t>net_dmz</t>
+  </si>
+  <si>
+    <t>192.168.99.0/24</t>
+  </si>
+  <si>
+    <t>192.168.10.0/24</t>
+  </si>
+  <si>
+    <t>192.168.1.0/24</t>
+  </si>
+  <si>
+    <t>192.168.100.0/24</t>
+  </si>
+  <si>
+    <t>syslog_server</t>
+  </si>
+  <si>
+    <t>snmp_server</t>
+  </si>
+  <si>
+    <t>flow_server</t>
+  </si>
+  <si>
+    <t>web_server1</t>
+  </si>
+  <si>
+    <t>ftp_server1</t>
+  </si>
+  <si>
+    <t>192.168.1.10/32</t>
+  </si>
+  <si>
+    <t>192.168.1.11/32</t>
+  </si>
+  <si>
+    <t>192.168.1.12/32</t>
+  </si>
+  <si>
+    <t>web_server2</t>
+  </si>
+  <si>
+    <t>web_servers</t>
+  </si>
+  <si>
+    <t>192.168.99.11/32</t>
+  </si>
+  <si>
+    <t>192.168.99.12/32</t>
+  </si>
+  <si>
+    <t>192.168.99.21/32</t>
+  </si>
+  <si>
+    <t>cust-http-dev</t>
+  </si>
+  <si>
+    <t>cust-https-dev</t>
+  </si>
+  <si>
+    <t>web-server-access-in</t>
+  </si>
+  <si>
+    <t>web-server-dev-access-in</t>
+  </si>
+  <si>
+    <t>ftp-access-in</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>log-access-in</t>
+  </si>
+  <si>
+    <t>mgmt_servers</t>
+  </si>
+  <si>
+    <t>cust-jflow</t>
+  </si>
+  <si>
+    <t>guest-access-out</t>
+  </si>
+  <si>
+    <t>mgmt-access-in</t>
+  </si>
+  <si>
+    <t>ssh-access-to-dmz</t>
+  </si>
+  <si>
+    <t>telnet-access-to-dmz</t>
+  </si>
+  <si>
+    <t>dmz-access-out</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Translated Address</t>
+  </si>
+  <si>
+    <t>Translated Port</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>default-source-net</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>203.0.0.1/32</t>
+  </si>
+  <si>
+    <t>mgmt-access-out</t>
+  </si>
+  <si>
+    <t>192.168.99.0.24</t>
+  </si>
+  <si>
+    <t>10.0.0.0/8</t>
+  </si>
+  <si>
+    <t>192.168.0.0/16</t>
+  </si>
+  <si>
+    <t>ten_eight</t>
+  </si>
+  <si>
+    <t>oneninetwo_six</t>
+  </si>
+  <si>
+    <t>oneseventwo-twelve</t>
+  </si>
+  <si>
+    <t>172.16.0.0/12</t>
+  </si>
+  <si>
+    <t>rfc1918</t>
+  </si>
+  <si>
+    <t>PBK_RTR1</t>
+  </si>
+  <si>
+    <t>Paperbark</t>
+  </si>
+  <si>
+    <t>junos-ftp-data</t>
+  </si>
+  <si>
+    <t>junos-finger</t>
+  </si>
+  <si>
+    <t>junos-biff</t>
+  </si>
+  <si>
+    <t>junos-bootpc</t>
+  </si>
+  <si>
+    <t>junos-bootps</t>
+  </si>
+  <si>
+    <t>junos-cvspserver</t>
+  </si>
+  <si>
+    <t>junos-dhcp-relay</t>
+  </si>
+  <si>
+    <t>junos-echo</t>
+  </si>
+  <si>
+    <t>junos-gopher</t>
+  </si>
+  <si>
+    <t>junos-http</t>
+  </si>
+  <si>
+    <t>junos-http-ext</t>
+  </si>
+  <si>
+    <t>junos-icmp-all</t>
+  </si>
+  <si>
+    <t>junos-imap</t>
+  </si>
+  <si>
+    <t>junos-l2tp</t>
+  </si>
+  <si>
+    <t>junos-ldap</t>
+  </si>
+  <si>
+    <t>junos-mail</t>
+  </si>
+  <si>
+    <t>junos-ms-rpc-tcp</t>
+  </si>
+  <si>
+    <t>junos-ms-rpc-udp</t>
+  </si>
+  <si>
+    <t>junos-ms-sql</t>
+  </si>
+  <si>
+    <t>junos-nbds</t>
+  </si>
+  <si>
+    <t>junos-nbname</t>
+  </si>
+  <si>
+    <t>junos-nfsd-tcp</t>
+  </si>
+  <si>
+    <t>junos-nfsd-udp</t>
+  </si>
+  <si>
+    <t>junos-nntp</t>
+  </si>
+  <si>
+    <t>junos-ping</t>
+  </si>
+  <si>
+    <t>junos-pop3</t>
+  </si>
+  <si>
+    <t>junos-pptp</t>
+  </si>
+  <si>
+    <t>junos-r2cp</t>
+  </si>
+  <si>
+    <t>junos-radius</t>
+  </si>
+  <si>
+    <t>junos-rtsp</t>
+  </si>
+  <si>
+    <t>junos-sccp</t>
+  </si>
+  <si>
+    <t>junos-smtp</t>
+  </si>
+  <si>
+    <t>junos-snpp</t>
+  </si>
+  <si>
+    <t>junos-syslog</t>
+  </si>
+  <si>
+    <t>junos-tacacs</t>
+  </si>
+  <si>
+    <t>junos-talk</t>
+  </si>
+  <si>
+    <t>junos-telnet</t>
+  </si>
+  <si>
+    <t>junos-tftp</t>
+  </si>
+  <si>
+    <t>junos-uucp</t>
+  </si>
+  <si>
+    <t>junos-wais</t>
+  </si>
+  <si>
+    <t>junos-winframe</t>
+  </si>
+  <si>
+    <t>Authentication Server Key</t>
+  </si>
+  <si>
+    <t>Super-User</t>
+  </si>
+  <si>
+    <t>key1234</t>
+  </si>
+  <si>
+    <t>192.168.1.13</t>
+  </si>
+  <si>
+    <t>Local Password Only</t>
+  </si>
+  <si>
+    <t>12/13</t>
+  </si>
+  <si>
+    <t>14/15</t>
+  </si>
+  <si>
+    <t>Empty-port 12</t>
+  </si>
+  <si>
+    <t>Empty-port 13</t>
+  </si>
+  <si>
+    <t>Empty-port 14</t>
+  </si>
+  <si>
+    <t>Empty-port 15</t>
+  </si>
+  <si>
     <t>PS 0
-(DC)</t>
+(AC)</t>
   </si>
   <si>
     <t>PS 1
-(DC)</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>memberOf</t>
-  </si>
-  <si>
-    <t>vrf</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>BrightNet</t>
-  </si>
-  <si>
-    <t>Gavin White</t>
-  </si>
-  <si>
-    <t>PO Box 143, Upper Coomera QLD 4209</t>
-  </si>
-  <si>
-    <t>1300 024 677</t>
-  </si>
-  <si>
-    <t>support@brightnet.com.au</t>
-  </si>
-  <si>
-    <t>SRX345</t>
-  </si>
-  <si>
-    <t>SD586932XT</t>
-  </si>
-  <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>Secondary</t>
-  </si>
-  <si>
-    <t>PBK_RTR2</t>
-  </si>
-  <si>
-    <t>SD586955PN</t>
-  </si>
-  <si>
-    <t>brightnet.com.au</t>
-  </si>
-  <si>
-    <t>1.1.1.1, 8.8.8.8</t>
-  </si>
-  <si>
-    <t>4.4.4.4</t>
-  </si>
-  <si>
-    <t>192.168.1.12</t>
-  </si>
-  <si>
-    <t>paperbark</t>
-  </si>
-  <si>
-    <t>192.168.1.11</t>
-  </si>
-  <si>
-    <t>192.168.1.10</t>
-  </si>
-  <si>
-    <t>ike</t>
-  </si>
-  <si>
-    <t>dmz</t>
-  </si>
-  <si>
-    <t>mgmt</t>
-  </si>
-  <si>
-    <t>ssh, ping</t>
-  </si>
-  <si>
-    <t>guest</t>
-  </si>
-  <si>
-    <t>ping</t>
-  </si>
-  <si>
-    <t>ge-0/0/1</t>
-  </si>
-  <si>
-    <t>ge-0/0/2</t>
-  </si>
-  <si>
-    <t>ge-0/0/4</t>
-  </si>
-  <si>
-    <t>DMZ Interface</t>
-  </si>
-  <si>
-    <t>Management Interface</t>
-  </si>
-  <si>
-    <t>Guest Network</t>
-  </si>
-  <si>
-    <t>Internal Network</t>
-  </si>
-  <si>
-    <t>192.168.100.1/24</t>
-  </si>
-  <si>
-    <t>192.168.10.1/24</t>
-  </si>
-  <si>
-    <t>192.168.1.1/24</t>
-  </si>
-  <si>
-    <t>192.168.99.1/24</t>
-  </si>
-  <si>
-    <t>net_mgmt</t>
-  </si>
-  <si>
-    <t>net_guest</t>
-  </si>
-  <si>
-    <t>net_internal</t>
-  </si>
-  <si>
-    <t>net_dmz</t>
-  </si>
-  <si>
-    <t>192.168.99.0/24</t>
-  </si>
-  <si>
-    <t>192.168.10.0/24</t>
-  </si>
-  <si>
-    <t>192.168.1.0/24</t>
-  </si>
-  <si>
-    <t>192.168.100.0/24</t>
-  </si>
-  <si>
-    <t>syslog_server</t>
-  </si>
-  <si>
-    <t>snmp_server</t>
-  </si>
-  <si>
-    <t>flow_server</t>
-  </si>
-  <si>
-    <t>web_server1</t>
-  </si>
-  <si>
-    <t>ftp_server1</t>
-  </si>
-  <si>
-    <t>192.168.1.10/32</t>
-  </si>
-  <si>
-    <t>192.168.1.11/32</t>
-  </si>
-  <si>
-    <t>192.168.1.12/32</t>
-  </si>
-  <si>
-    <t>web_server2</t>
-  </si>
-  <si>
-    <t>web_servers</t>
-  </si>
-  <si>
-    <t>192.168.99.11/32</t>
-  </si>
-  <si>
-    <t>192.168.99.12/32</t>
-  </si>
-  <si>
-    <t>192.168.99.21/32</t>
-  </si>
-  <si>
-    <t>cust-http-dev</t>
-  </si>
-  <si>
-    <t>cust-https-dev</t>
-  </si>
-  <si>
-    <t>web-server-access-in</t>
-  </si>
-  <si>
-    <t>web-server-dev-access-in</t>
-  </si>
-  <si>
-    <t>ftp-access-in</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>log-access-in</t>
-  </si>
-  <si>
-    <t>mgmt_servers</t>
-  </si>
-  <si>
-    <t>cust-jflow</t>
-  </si>
-  <si>
-    <t>guest-access-out</t>
-  </si>
-  <si>
-    <t>mgmt-access-in</t>
-  </si>
-  <si>
-    <t>ssh-access-to-dmz</t>
-  </si>
-  <si>
-    <t>telnet-access-to-dmz</t>
-  </si>
-  <si>
-    <t>dmz-access-out</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Translated Address</t>
-  </si>
-  <si>
-    <t>Translated Port</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>default-source-net</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>203.0.0.1/32</t>
-  </si>
-  <si>
-    <t>mgmt-access-out</t>
-  </si>
-  <si>
-    <t>192.168.99.0.24</t>
-  </si>
-  <si>
-    <t>10.0.0.0/8</t>
-  </si>
-  <si>
-    <t>192.168.0.0/16</t>
-  </si>
-  <si>
-    <t>ten_eight</t>
-  </si>
-  <si>
-    <t>oneninetwo_six</t>
-  </si>
-  <si>
-    <t>oneseventwo-twelve</t>
-  </si>
-  <si>
-    <t>172.16.0.0/12</t>
-  </si>
-  <si>
-    <t>rfc1918</t>
-  </si>
-  <si>
-    <t>PBK_RTR1</t>
-  </si>
-  <si>
-    <t>Paperbark</t>
-  </si>
-  <si>
-    <t>junos-ftp-data</t>
-  </si>
-  <si>
-    <t>junos-finger</t>
-  </si>
-  <si>
-    <t>junos-biff</t>
-  </si>
-  <si>
-    <t>junos-bootpc</t>
-  </si>
-  <si>
-    <t>junos-bootps</t>
-  </si>
-  <si>
-    <t>junos-cvspserver</t>
-  </si>
-  <si>
-    <t>junos-dhcp-relay</t>
-  </si>
-  <si>
-    <t>junos-echo</t>
-  </si>
-  <si>
-    <t>junos-gopher</t>
-  </si>
-  <si>
-    <t>junos-http</t>
-  </si>
-  <si>
-    <t>junos-http-ext</t>
-  </si>
-  <si>
-    <t>junos-icmp-all</t>
-  </si>
-  <si>
-    <t>junos-imap</t>
-  </si>
-  <si>
-    <t>junos-l2tp</t>
-  </si>
-  <si>
-    <t>junos-ldap</t>
-  </si>
-  <si>
-    <t>junos-mail</t>
-  </si>
-  <si>
-    <t>junos-ms-rpc-tcp</t>
-  </si>
-  <si>
-    <t>junos-ms-rpc-udp</t>
-  </si>
-  <si>
-    <t>junos-ms-sql</t>
-  </si>
-  <si>
-    <t>junos-nbds</t>
-  </si>
-  <si>
-    <t>junos-nbname</t>
-  </si>
-  <si>
-    <t>junos-nfsd-tcp</t>
-  </si>
-  <si>
-    <t>junos-nfsd-udp</t>
-  </si>
-  <si>
-    <t>junos-nntp</t>
-  </si>
-  <si>
-    <t>junos-ping</t>
-  </si>
-  <si>
-    <t>junos-pop3</t>
-  </si>
-  <si>
-    <t>junos-pptp</t>
-  </si>
-  <si>
-    <t>junos-r2cp</t>
-  </si>
-  <si>
-    <t>junos-radius</t>
-  </si>
-  <si>
-    <t>junos-rtsp</t>
-  </si>
-  <si>
-    <t>junos-sccp</t>
-  </si>
-  <si>
-    <t>junos-smtp</t>
-  </si>
-  <si>
-    <t>junos-snpp</t>
-  </si>
-  <si>
-    <t>junos-syslog</t>
-  </si>
-  <si>
-    <t>junos-tacacs</t>
-  </si>
-  <si>
-    <t>junos-talk</t>
-  </si>
-  <si>
-    <t>junos-telnet</t>
-  </si>
-  <si>
-    <t>junos-tftp</t>
-  </si>
-  <si>
-    <t>junos-uucp</t>
-  </si>
-  <si>
-    <t>junos-wais</t>
-  </si>
-  <si>
-    <t>junos-winframe</t>
-  </si>
-  <si>
-    <t>Authentication Server Key</t>
-  </si>
-  <si>
-    <t>Super-User</t>
-  </si>
-  <si>
-    <t>key1234</t>
-  </si>
-  <si>
-    <t>192.168.1.13</t>
-  </si>
-  <si>
-    <t>Local Password Only</t>
+(AC)</t>
   </si>
 </sst>
 </file>
@@ -2837,7 +2855,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -3023,17 +3041,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -3414,7 +3421,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3454,77 +3461,76 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3538,7 +3544,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3551,10 +3557,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3563,7 +3569,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3584,29 +3590,32 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3614,22 +3623,19 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4324,36 +4330,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="58" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>656</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>720</v>
-      </c>
-      <c r="C2" s="61"/>
+        <v>718</v>
+      </c>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>274</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="C3" s="61"/>
+        <v>805</v>
+      </c>
+      <c r="C3" s="60"/>
     </row>
     <row r="4" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>722</v>
+      <c r="B4" s="53" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4361,7 +4367,7 @@
         <v>276</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -4370,7 +4376,7 @@
         <v>277</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>654</v>
@@ -4380,8 +4386,8 @@
       <c r="A7" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="53" t="s">
-        <v>724</v>
+      <c r="B7" s="52" t="s">
+        <v>722</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>655</v>
@@ -4393,21 +4399,21 @@
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="59" t="s">
         <v>653</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>273</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4415,10 +4421,10 @@
         <v>281</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4426,10 +4432,10 @@
         <v>280</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4437,10 +4443,10 @@
         <v>652</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4449,10 +4455,10 @@
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="58" t="s">
         <v>282</v>
       </c>
-      <c r="B15" s="59"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4460,7 +4466,7 @@
         <v>283</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -4469,7 +4475,7 @@
         <v>284</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -4487,7 +4493,7 @@
         <v>285</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C19" s="5"/>
     </row>
@@ -4505,7 +4511,7 @@
         <v>644</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -4514,7 +4520,7 @@
         <v>645</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -4523,7 +4529,7 @@
         <v>287</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -4532,7 +4538,7 @@
         <v>646</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -4542,10 +4548,10 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="58" t="s">
         <v>657</v>
       </c>
-      <c r="B26" s="59"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4553,7 +4559,7 @@
         <v>658</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -4562,7 +4568,7 @@
         <v>661</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -4571,32 +4577,32 @@
         <v>659</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>660</v>
       </c>
-      <c r="B30" s="58">
+      <c r="B30" s="57">
         <v>1812</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>849</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>851</v>
-      </c>
       <c r="C31" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="58" t="s">
         <v>650</v>
       </c>
-      <c r="B33" s="59"/>
+      <c r="B33" s="58"/>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7039,92 +7045,92 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="G5" s="56"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="G6" s="56"/>
+      <c r="A6" s="55"/>
+      <c r="G6" s="55"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="G7" s="56"/>
+      <c r="A7" s="55"/>
+      <c r="G7" s="55"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="G8" s="56"/>
+      <c r="A8" s="55"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="G9" s="56"/>
+      <c r="A9" s="55"/>
+      <c r="G9" s="55"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="G10" s="56"/>
+      <c r="A10" s="55"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="G11" s="56"/>
+      <c r="A11" s="55"/>
+      <c r="G11" s="55"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="G12" s="56"/>
+      <c r="A12" s="55"/>
+      <c r="G12" s="55"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="G13" s="56"/>
+      <c r="A13" s="55"/>
+      <c r="G13" s="55"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="G14" s="56"/>
+      <c r="A14" s="55"/>
+      <c r="G14" s="55"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="A15" s="55"/>
+      <c r="G15" s="55"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="A16" s="55"/>
+      <c r="G16" s="55"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
-      <c r="G17" s="56"/>
+      <c r="A17" s="55"/>
+      <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
-      <c r="G18" s="56"/>
+      <c r="A18" s="55"/>
+      <c r="G18" s="55"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
-      <c r="G19" s="56"/>
+      <c r="A19" s="55"/>
+      <c r="G19" s="55"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="G20" s="56"/>
+      <c r="A20" s="55"/>
+      <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
-      <c r="G21" s="56"/>
+      <c r="A21" s="55"/>
+      <c r="G21" s="55"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
+      <c r="A22" s="55"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
+      <c r="A23" s="55"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
+      <c r="A24" s="55"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
+      <c r="A25" s="55"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
+      <c r="A26" s="55"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
+      <c r="A27" s="55"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
+      <c r="A28" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7136,7 +7142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B921653-A31E-4A4F-AA14-15BAA78797BE}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -7155,11 +7161,11 @@
       <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7170,7 +7176,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7182,36 +7188,36 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -7331,7 +7337,7 @@
       <c r="G1" t="s">
         <v>261</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7358,18 +7364,18 @@
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D3" t="s">
         <v>268</v>
@@ -7378,10 +7384,10 @@
         <v>271</v>
       </c>
       <c r="F3" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -7392,13 +7398,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D6" t="s">
         <v>268</v>
@@ -7407,7 +7413,7 @@
         <v>271</v>
       </c>
       <c r="F6" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
@@ -7415,13 +7421,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D7" t="s">
         <v>268</v>
@@ -7430,13 +7436,13 @@
         <v>271</v>
       </c>
       <c r="F7" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="G7" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="H7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7444,13 +7450,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D9" t="s">
         <v>268</v>
@@ -7459,10 +7465,10 @@
         <v>271</v>
       </c>
       <c r="F9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7633,7 +7639,7 @@
         <v>261</v>
       </c>
       <c r="D1" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7649,32 +7655,32 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B3" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C3" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B4" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C4" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -7682,157 +7688,157 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B6" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D7" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B8" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C8" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D8" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B10" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C10" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D10" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B11" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C11" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C13" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C14" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B15" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C15" t="s">
         <v>259</v>
       </c>
       <c r="D15" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B16" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C16" t="s">
         <v>259</v>
       </c>
       <c r="D16" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B17" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C17" t="s">
         <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C18" t="s">
         <v>259</v>
@@ -7915,7 +7921,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -7926,7 +7932,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -7937,7 +7943,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -7964,7 +7970,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -7986,7 +7992,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -8047,7 +8053,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -8058,7 +8064,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -8083,7 +8089,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -8108,7 +8114,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -8143,7 +8149,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -8154,7 +8160,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -8176,7 +8182,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B29" t="s">
         <v>83</v>
@@ -8295,7 +8301,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
@@ -8345,7 +8351,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
@@ -8356,7 +8362,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -8400,7 +8406,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -8494,7 +8500,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
@@ -8508,7 +8514,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
@@ -8602,7 +8608,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
@@ -8624,7 +8630,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B91" t="s">
         <v>4</v>
@@ -8635,7 +8641,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B92" t="s">
         <v>4</v>
@@ -8668,7 +8674,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
@@ -8679,7 +8685,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B96" t="s">
         <v>4</v>
@@ -8690,7 +8696,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
@@ -8780,7 +8786,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B106" t="s">
         <v>83</v>
@@ -8793,7 +8799,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B108" t="s">
         <v>5</v>
@@ -8821,7 +8827,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
@@ -8846,7 +8852,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B112" t="s">
         <v>4</v>
@@ -8868,7 +8874,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B114" t="s">
         <v>4</v>
@@ -8934,7 +8940,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -8948,7 +8954,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
@@ -8997,7 +9003,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
@@ -9027,7 +9033,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -9395,7 +9401,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B178" t="s">
         <v>4</v>
@@ -9406,7 +9412,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B179" t="s">
         <v>5</v>
@@ -9428,7 +9434,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B181" t="s">
         <v>208</v>
@@ -9450,7 +9456,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B183" t="s">
         <v>5</v>
@@ -9461,7 +9467,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B184" t="s">
         <v>4</v>
@@ -9497,7 +9503,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B187" t="s">
         <v>4</v>
@@ -9541,7 +9547,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="B191" t="s">
         <v>5</v>
@@ -9574,7 +9580,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B194" t="s">
         <v>5</v>
@@ -9634,7 +9640,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="9" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B200" s="9" t="s">
         <v>5</v>
@@ -9646,7 +9652,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="9" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B201" s="9" t="s">
         <v>5</v>
@@ -9658,7 +9664,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="9" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B202" s="9" t="s">
         <v>4</v>
@@ -11576,10 +11582,10 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C3" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -11588,7 +11594,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G3" t="s">
         <v>107</v>
@@ -11611,10 +11617,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C4" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -11623,7 +11629,7 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G4" t="s">
         <v>108</v>
@@ -11646,19 +11652,19 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G5" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="H5" t="s">
         <v>95</v>
@@ -11675,19 +11681,19 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C6" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G6" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="H6" t="s">
         <v>95</v>
@@ -11698,19 +11704,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E7" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F7" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G7" t="s">
         <v>144</v>
@@ -11727,10 +11733,10 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -11739,7 +11745,7 @@
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="G8" t="s">
         <v>103</v>
@@ -11754,7 +11760,7 @@
         <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M8" t="s">
         <v>19</v>
@@ -11762,19 +11768,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C9" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E9" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -11791,10 +11797,10 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C10" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -11803,7 +11809,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="G10" t="s">
         <v>104</v>
@@ -11818,7 +11824,7 @@
         <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M10" t="s">
         <v>19</v>
@@ -11826,22 +11832,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C11" t="s">
+        <v>780</v>
+      </c>
+      <c r="E11" t="s">
+        <v>770</v>
+      </c>
+      <c r="F11" t="s">
+        <v>781</v>
+      </c>
+      <c r="G11" t="s">
         <v>782</v>
-      </c>
-      <c r="E11" t="s">
-        <v>772</v>
-      </c>
-      <c r="F11" t="s">
-        <v>783</v>
-      </c>
-      <c r="G11" t="s">
-        <v>784</v>
       </c>
       <c r="H11" t="s">
         <v>95</v>
@@ -11852,16 +11858,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E12" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -11878,16 +11884,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B13" t="s">
         <v>259</v>
       </c>
       <c r="C13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E13" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -11907,16 +11913,16 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C14" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E14" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F14" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -11933,16 +11939,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C15" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E15" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F15" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G15" t="s">
         <v>147</v>
@@ -11951,21 +11957,21 @@
         <v>95</v>
       </c>
       <c r="M15" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E16" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -11982,16 +11988,16 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E17" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -12008,16 +12014,16 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E18" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -12096,7 +12102,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>263</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -12112,13 +12118,13 @@
         <v>8</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>788</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>789</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>790</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>791</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>792</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>15</v>
@@ -12126,7 +12132,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -12135,7 +12141,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F2" t="s">
         <v>94</v>
@@ -12149,25 +12155,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D3" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G3" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="H3">
         <v>80</v>
@@ -12178,25 +12184,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D4" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G4" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="H4">
         <v>443</v>
@@ -12207,22 +12213,22 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F5" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G5" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="H5">
         <v>8080</v>
@@ -12233,22 +12239,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D6" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F6" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G6" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="H6">
         <v>8443</v>
@@ -12259,45 +12265,45 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F8" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G8" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="H8">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B10" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F10" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="G10" t="s">
         <v>265</v>
@@ -12308,19 +12314,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B11" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F11" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G11" t="s">
         <v>265</v>
@@ -12331,19 +12337,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F12" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G12" t="s">
         <v>265</v>
@@ -12389,30 +12395,30 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD20"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="51" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="14" width="14.28515625" customWidth="1"/>
-    <col min="15" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="4.7109375" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" customWidth="1"/>
-    <col min="30" max="30" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="29" width="4.7109375" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="32" max="32" width="5.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
-        <v>714</v>
+    <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
+        <v>858</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>663</v>
@@ -12421,42 +12427,46 @@
         <f ca="1">MID(CELL("filename",D1),FIND("]",CELL("filename",D1))+1,11)</f>
         <v>srx1600-phy</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>664</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="69"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="68"/>
+    </row>
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64"/>
       <c r="B2" s="13" t="s">
         <v>665</v>
       </c>
       <c r="C2" s="15"/>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="66" t="s">
         <v>666</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="69"/>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="68"/>
+    </row>
+    <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="64"/>
       <c r="B3" s="13" t="s">
         <v>667</v>
       </c>
@@ -12481,252 +12491,276 @@
       <c r="I3" s="19" t="s">
         <v>674</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
+        <v>852</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>853</v>
+      </c>
+      <c r="L3" s="20" t="s">
         <v>669</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>669</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>670</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
-    </row>
-    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="22"/>
+    </row>
+    <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="65"/>
       <c r="B4" s="13" t="s">
         <v>675</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>676</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="69" t="s">
         <v>664</v>
       </c>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="72"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
-        <v>715</v>
-      </c>
-      <c r="B5" s="73" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="71"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>859</v>
+      </c>
+      <c r="B5" s="72" t="s">
         <v>677</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="81" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="80" t="s">
         <v>678</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="24" t="s">
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="23" t="s">
         <v>679</v>
       </c>
-      <c r="K5" s="84" t="s">
+      <c r="M5" s="83" t="s">
         <v>680</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="25" t="s">
+      <c r="N5" s="84"/>
+      <c r="O5" s="24" t="s">
         <v>681</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="P5" s="24" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="86" t="s">
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="64"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="85" t="s">
         <v>683</v>
       </c>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="26" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="25" t="s">
         <v>684</v>
       </c>
-      <c r="K6" s="62" t="s">
+      <c r="M6" s="61" t="s">
         <v>685</v>
       </c>
-      <c r="L6" s="63"/>
-      <c r="M6" s="27" t="s">
+      <c r="N6" s="62"/>
+      <c r="O6" s="26" t="s">
         <v>686</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="P6" s="26" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="28" t="s">
+    <row r="7" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="64"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="27" t="s">
         <v>688</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>690</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>691</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="29" t="s">
         <v>692</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>693</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="29" t="s">
+        <v>854</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>856</v>
+      </c>
+      <c r="L7" s="30" t="s">
         <v>688</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="M7" s="31" t="s">
         <v>688</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="N7" s="32" t="s">
         <v>689</v>
       </c>
-      <c r="M7" s="34" t="s">
+      <c r="O7" s="33" t="s">
         <v>694</v>
       </c>
-      <c r="N7" s="34" t="s">
+      <c r="P7" s="33" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="66"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="35" t="s">
+    <row r="8" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="65"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="34" t="s">
         <v>696</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="35" t="s">
         <v>697</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="35" t="s">
         <v>698</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="36" t="s">
         <v>699</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="36" t="s">
         <v>700</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="36" t="s">
         <v>701</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="36" t="s">
+        <v>855</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>857</v>
+      </c>
+      <c r="L8" s="37" t="s">
         <v>696</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="M8" s="38" t="s">
         <v>696</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="N8" s="39" t="s">
         <v>697</v>
       </c>
-      <c r="M8" s="41" t="s">
+      <c r="O8" s="40" t="s">
         <v>694</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="P8" s="41" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9"/>
       <c r="C9"/>
-      <c r="AD9" s="43"/>
-    </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF9" s="42"/>
+    </row>
+    <row r="10" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10"/>
       <c r="C10" s="13" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B11"/>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="43" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B12"/>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B13"/>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="45" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="46" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B15"/>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16"/>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="37" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="47" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="49" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="20" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="50" t="s">
         <v>713</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="D1:P1"/>
+    <mergeCell ref="D2:P2"/>
+    <mergeCell ref="D4:P4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="D6:K6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="62" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Dynamic Application processing
</commit_message>
<xml_diff>
--- a/excel_templates/sample_workbook.xlsx
+++ b/excel_templates/sample_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewh\Dropbox\Gav\My Documents\Juniper Scripts\junos-config-templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2623851D-8719-450D-8C74-4C9C3ACA6A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335A150E-3E0D-497A-A881-3E41ABAD20DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25320" yWindow="450" windowWidth="32460" windowHeight="20880" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
+    <workbookView xWindow="1560" yWindow="720" windowWidth="22245" windowHeight="20880" activeTab="6" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9771" uniqueCount="9128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9780" uniqueCount="9134">
   <si>
     <t>Name</t>
   </si>
@@ -27495,6 +27495,24 @@
   </si>
   <si>
     <t xml:space="preserve">       Multiple entries for the same policy must have exactly the same policy-name.</t>
+  </si>
+  <si>
+    <t>reth0</t>
+  </si>
+  <si>
+    <t>aggregate</t>
+  </si>
+  <si>
+    <t>agg-member</t>
+  </si>
+  <si>
+    <t>ge-0/0/5</t>
+  </si>
+  <si>
+    <t>Aggregate member interface 1</t>
+  </si>
+  <si>
+    <t>Aggregate member interface 2</t>
   </si>
 </sst>
 </file>
@@ -27705,7 +27723,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -27755,9 +27773,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -28444,7 +28459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68590D1-FAE6-4DDC-BE52-A7BC10F9195F}">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -29589,21 +29604,21 @@
       <c r="T54" s="24"/>
     </row>
     <row r="55" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H55" s="25" t="s">
+      <c r="H55" s="24" t="s">
         <v>9113</v>
       </c>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="25"/>
-      <c r="T55" s="25"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="24"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="24"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="24"/>
+      <c r="T55" s="24"/>
     </row>
     <row r="56" spans="7:20" x14ac:dyDescent="0.25">
       <c r="H56" s="24" t="s">
@@ -30346,7 +30361,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30445,49 +30460,36 @@
       <c r="A6" t="s">
         <v>687</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>691</v>
+        <v>9132</v>
       </c>
       <c r="D6" t="s">
         <v>263</v>
       </c>
       <c r="E6" t="s">
-        <v>266</v>
-      </c>
-      <c r="F6" t="s">
-        <v>693</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
+        <v>9130</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>687</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
+        <v>9131</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>690</v>
+        <v>9133</v>
       </c>
       <c r="D7" t="s">
         <v>263</v>
       </c>
       <c r="E7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" t="s">
-        <v>692</v>
-      </c>
-      <c r="G7" t="s">
-        <v>683</v>
-      </c>
-      <c r="H7" t="s">
-        <v>684</v>
+        <v>9130</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -30495,35 +30497,78 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>686</v>
+        <v>9128</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>9129</v>
       </c>
       <c r="E9" t="s">
         <v>266</v>
       </c>
       <c r="F9" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G9" t="s">
-        <v>681</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+      <c r="A10" t="s">
+        <v>9128</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>690</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" t="s">
+        <v>692</v>
+      </c>
+      <c r="G10" t="s">
+        <v>683</v>
+      </c>
+      <c r="H10" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="A12" t="s">
+        <v>686</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>689</v>
+      </c>
+      <c r="D12" t="s">
+        <v>263</v>
+      </c>
+      <c r="E12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F12" t="s">
+        <v>694</v>
+      </c>
+      <c r="G12" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
@@ -34566,8 +34611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3361E218-E961-466F-899C-D4E612D4BCFC}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34952,6 +34997,9 @@
       <c r="H12" t="s">
         <v>95</v>
       </c>
+      <c r="L12" t="s">
+        <v>4908</v>
+      </c>
       <c r="M12" t="s">
         <v>19</v>
       </c>
@@ -35113,7 +35161,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M200 I2:K200" xr:uid="{20F659FA-539B-45DF-B34F-F8E309AFB81C}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
@@ -35124,20 +35172,14 @@
       <formula1>1</formula1>
       <formula2>999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F200" xr:uid="{48EFB17C-041E-420E-8E56-38BCA49AEA5D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F200" xr:uid="{48EFB17C-041E-420E-8E56-38BCA49AEA5D}">
       <formula1>objects_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B200" xr:uid="{8A49BAA3-B996-493E-BA71-0F54E045024D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:B200" xr:uid="{8A49BAA3-B996-493E-BA71-0F54E045024D}">
       <formula1>zones_list</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G200" xr:uid="{4E7D6E73-8ECC-4669-86A7-D3AF53E627C9}">
       <formula1>apps_list</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A200" xr:uid="{B5584CD6-747F-4219-BA04-C832BC308B8B}">
-      <formula1>zones_list</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E200" xr:uid="{3E70D3FD-A800-4A87-BE13-450D52851199}">
-      <formula1>objects_list</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L200" xr:uid="{79F49256-A37D-4931-BE11-528E3B0614AD}">
       <formula1>dynapps_list</formula1>
@@ -35427,7 +35469,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E200" xr:uid="{B070D166-E21C-44DD-B082-A77269BA2C59}">
       <formula1>1</formula1>
       <formula2>999</formula2>
@@ -35438,10 +35480,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A200" xr:uid="{0598ABBA-CAE4-49B2-8150-57BBF82F22A6}">
       <formula1>"Source, Destination, Static"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C200" xr:uid="{44ED0A2A-ABB4-4F36-AD3A-B1B7427AE46C}">
-      <formula1>zones_list</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B200" xr:uid="{F1E693EE-BEB0-4009-A6EB-89BC984D068C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C200" xr:uid="{44ED0A2A-ABB4-4F36-AD3A-B1B7427AE46C}">
       <formula1>zones_list</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add description for NAT Rules
</commit_message>
<xml_diff>
--- a/excel_templates/sample_workbook.xlsx
+++ b/excel_templates/sample_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewh\Dropbox\Gav\My Documents\Juniper Scripts\junos-config-templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335A150E-3E0D-497A-A881-3E41ABAD20DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D643DB50-FBFF-45BB-A32E-609E083D2858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="720" windowWidth="22245" windowHeight="20880" activeTab="6" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
+    <workbookView xWindow="3510" yWindow="720" windowWidth="38565" windowHeight="20880" activeTab="7" xr2:uid="{77295D64-946B-4548-9E73-765B9A5FEEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9780" uniqueCount="9134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9781" uniqueCount="9134">
   <si>
     <t>Name</t>
   </si>
@@ -27723,7 +27723,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -27759,6 +27759,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -27768,15 +27777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
@@ -28123,9 +28124,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FDCF5AD-E100-4012-9806-A624A022335C}" name="Table73" displayName="Table73" ref="A1:I200" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:I200" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FDCF5AD-E100-4012-9806-A624A022335C}" name="Table73" displayName="Table73" ref="A1:J200" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:J200" xr:uid="{A7AF67BF-7C87-4A66-B6AD-0F0513CB95A4}"/>
+  <tableColumns count="10">
     <tableColumn id="14" xr3:uid="{6C4F03B8-D3CF-4725-AB73-216B28241D58}" name="Type"/>
     <tableColumn id="1" xr3:uid="{74FC297E-1796-4A86-A996-88558EF7436E}" name="From Zone"/>
     <tableColumn id="2" xr3:uid="{573E93E3-03FD-42E9-ACDB-12260419E3FE}" name="To Zone"/>
@@ -28135,6 +28136,7 @@
     <tableColumn id="6" xr3:uid="{9C4C72C3-B8D1-496B-ADC5-F0BC62F14F51}" name="Translated Address"/>
     <tableColumn id="7" xr3:uid="{9B3AEF9B-2886-4E83-AB28-18E040684FED}" name="Translated Port"/>
     <tableColumn id="13" xr3:uid="{BDA12309-DEBF-4CB7-A906-6EB90E9A6DE7}" name="Enabled"/>
+    <tableColumn id="8" xr3:uid="{80CCCF8E-4530-4FA0-AFBA-D9271B8848C2}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28471,11 +28473,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -28484,7 +28486,7 @@
       <c r="B2" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -28493,7 +28495,7 @@
       <c r="B3" s="7" t="s">
         <v>747</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -28502,22 +28504,22 @@
       <c r="B4" s="14" t="s">
         <v>663</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="20" t="s">
         <v>9078</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -28538,22 +28540,22 @@
       <c r="C6" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="19" t="s">
         <v>9080</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -28565,66 +28567,66 @@
       <c r="C7" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="21" t="s">
         <v>9081</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="19" t="s">
         <v>9079</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="23" t="s">
         <v>648</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="G9" s="24" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="G9" s="19" t="s">
         <v>9083</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -28636,21 +28638,21 @@
       <c r="C10" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="19" t="s">
         <v>9084</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -28662,21 +28664,21 @@
       <c r="C11" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="19" t="s">
         <v>9085</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -28688,21 +28690,21 @@
       <c r="C12" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="19" t="s">
         <v>9087</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -28714,63 +28716,63 @@
       <c r="C13" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="19" t="s">
         <v>9086</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="19" t="s">
         <v>9088</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="5"/>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="19" t="s">
         <v>9089</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -28780,22 +28782,22 @@
         <v>672</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="19" t="s">
         <v>9082</v>
       </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -28805,21 +28807,21 @@
         <v>673</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="19" t="s">
         <v>9090</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -28829,21 +28831,21 @@
         <v>526</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="19" t="s">
         <v>9091</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -28853,21 +28855,21 @@
         <v>674</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="19" t="s">
         <v>9092</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -28877,21 +28879,21 @@
         <v>2</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="19" t="s">
         <v>9093</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -28901,22 +28903,22 @@
         <v>675</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="19" t="s">
         <v>9094</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -28926,21 +28928,21 @@
         <v>676</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="19" t="s">
         <v>9096</v>
       </c>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -28950,21 +28952,21 @@
         <v>678</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="19" t="s">
         <v>9097</v>
       </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -28974,63 +28976,63 @@
         <v>677</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="19" t="s">
         <v>9098</v>
       </c>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="19" t="s">
         <v>9099</v>
       </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="22" t="s">
         <v>652</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="5"/>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="19" t="s">
         <v>9100</v>
       </c>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -29040,21 +29042,21 @@
         <v>793</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="19" t="s">
         <v>9101</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -29064,21 +29066,21 @@
         <v>790</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="19" t="s">
         <v>9095</v>
       </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -29087,22 +29089,22 @@
       <c r="B29" s="7" t="s">
         <v>792</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="19" t="s">
         <v>9102</v>
       </c>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -29112,21 +29114,21 @@
         <v>1812</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="19" t="s">
         <v>9103</v>
       </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -29136,60 +29138,60 @@
         <v>791</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="H31" s="24" t="s">
+      <c r="H31" s="19" t="s">
         <v>9104</v>
       </c>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H32" s="24" t="s">
+      <c r="H32" s="19" t="s">
         <v>9105</v>
       </c>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="22" t="s">
         <v>645</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="5"/>
-      <c r="H33" s="24" t="s">
+      <c r="H33" s="19" t="s">
         <v>9106</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -29197,22 +29199,22 @@
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
-      <c r="G34" s="24" t="s">
+      <c r="G34" s="19" t="s">
         <v>9119</v>
       </c>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="24"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -29220,21 +29222,21 @@
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
-      <c r="H35" s="24" t="s">
+      <c r="H35" s="19" t="s">
         <v>9107</v>
       </c>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="24"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -29242,21 +29244,21 @@
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
-      <c r="H36" s="24" t="s">
+      <c r="H36" s="19" t="s">
         <v>9111</v>
       </c>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -29264,21 +29266,21 @@
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
-      <c r="H37" s="24" t="s">
+      <c r="H37" s="19" t="s">
         <v>9110</v>
       </c>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="24"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -29286,21 +29288,21 @@
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="19" t="s">
         <v>9108</v>
       </c>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="24"/>
-      <c r="T38" s="24"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -29308,21 +29310,21 @@
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
-      <c r="H39" s="24" t="s">
+      <c r="H39" s="19" t="s">
         <v>9112</v>
       </c>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="24"/>
-      <c r="O39" s="24"/>
-      <c r="P39" s="24"/>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="24"/>
-      <c r="S39" s="24"/>
-      <c r="T39" s="24"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -29330,22 +29332,22 @@
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
-      <c r="G40" s="24" t="s">
+      <c r="G40" s="19" t="s">
         <v>9120</v>
       </c>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="24"/>
-      <c r="T40" s="24"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
@@ -29353,21 +29355,21 @@
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="5"/>
-      <c r="H41" s="24" t="s">
+      <c r="H41" s="19" t="s">
         <v>9109</v>
       </c>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="24"/>
-      <c r="S41" s="24"/>
-      <c r="T41" s="24"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
@@ -29375,21 +29377,21 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="5"/>
-      <c r="H42" s="24" t="s">
+      <c r="H42" s="19" t="s">
         <v>9124</v>
       </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
-      <c r="P42" s="24"/>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="24"/>
-      <c r="S42" s="24"/>
-      <c r="T42" s="24"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
@@ -29399,301 +29401,310 @@
         <v>15</v>
       </c>
       <c r="C43" s="5"/>
-      <c r="H43" s="24" t="s">
+      <c r="H43" s="19" t="s">
         <v>9115</v>
       </c>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="24"/>
-      <c r="P43" s="24"/>
-      <c r="Q43" s="24"/>
-      <c r="R43" s="24"/>
-      <c r="S43" s="24"/>
-      <c r="T43" s="24"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H44" s="24" t="s">
+      <c r="H44" s="19" t="s">
         <v>9113</v>
       </c>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="24"/>
-      <c r="P44" s="24"/>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="24"/>
-      <c r="S44" s="24"/>
-      <c r="T44" s="24"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H45" s="24" t="s">
+      <c r="H45" s="19" t="s">
         <v>9127</v>
       </c>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="24"/>
-      <c r="P45" s="24"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="24"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H46" s="24" t="s">
+      <c r="H46" s="19" t="s">
         <v>9114</v>
       </c>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="24"/>
-      <c r="P46" s="24"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
-      <c r="T46" s="24"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="19" t="s">
         <v>9116</v>
       </c>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="24"/>
-      <c r="P47" s="24"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="24"/>
-      <c r="S47" s="24"/>
-      <c r="T47" s="24"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H48" s="24" t="s">
+      <c r="H48" s="19" t="s">
         <v>9118</v>
       </c>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="24"/>
-      <c r="S48" s="24"/>
-      <c r="T48" s="24"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
     </row>
     <row r="49" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H49" s="24" t="s">
+      <c r="H49" s="19" t="s">
         <v>9117</v>
       </c>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="24"/>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="24"/>
-      <c r="P49" s="24"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="24"/>
-      <c r="S49" s="24"/>
-      <c r="T49" s="24"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="19"/>
+      <c r="T49" s="19"/>
     </row>
     <row r="50" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G50" s="24" t="s">
+      <c r="G50" s="19" t="s">
         <v>9121</v>
       </c>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
-      <c r="P50" s="24"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-      <c r="T50" s="24"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
     </row>
     <row r="51" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H51" s="24" t="s">
+      <c r="H51" s="19" t="s">
         <v>9123</v>
       </c>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="24"/>
-      <c r="T51" s="24"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="19"/>
+      <c r="T51" s="19"/>
     </row>
     <row r="52" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H52" s="24" t="s">
+      <c r="H52" s="19" t="s">
         <v>9122</v>
       </c>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="24"/>
-      <c r="S52" s="24"/>
-      <c r="T52" s="24"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="19"/>
+      <c r="T52" s="19"/>
     </row>
     <row r="53" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H53" s="24" t="s">
+      <c r="H53" s="19" t="s">
         <v>9125</v>
       </c>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="24"/>
-      <c r="O53" s="24"/>
-      <c r="P53" s="24"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="24"/>
-      <c r="S53" s="24"/>
-      <c r="T53" s="24"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="19"/>
+      <c r="T53" s="19"/>
     </row>
     <row r="54" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H54" s="24" t="s">
+      <c r="H54" s="19" t="s">
         <v>9126</v>
       </c>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="24"/>
-      <c r="O54" s="24"/>
-      <c r="P54" s="24"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="24"/>
-      <c r="S54" s="24"/>
-      <c r="T54" s="24"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="19"/>
+      <c r="S54" s="19"/>
+      <c r="T54" s="19"/>
     </row>
     <row r="55" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H55" s="24" t="s">
+      <c r="H55" s="19" t="s">
         <v>9113</v>
       </c>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="24"/>
-      <c r="N55" s="24"/>
-      <c r="O55" s="24"/>
-      <c r="P55" s="24"/>
-      <c r="Q55" s="24"/>
-      <c r="R55" s="24"/>
-      <c r="S55" s="24"/>
-      <c r="T55" s="24"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+      <c r="P55" s="19"/>
+      <c r="Q55" s="19"/>
+      <c r="R55" s="19"/>
+      <c r="S55" s="19"/>
+      <c r="T55" s="19"/>
     </row>
     <row r="56" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H56" s="24" t="s">
+      <c r="H56" s="19" t="s">
         <v>9127</v>
       </c>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24"/>
-      <c r="K56" s="24"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="24"/>
-      <c r="N56" s="24"/>
-      <c r="O56" s="24"/>
-      <c r="P56" s="24"/>
-      <c r="Q56" s="24"/>
-      <c r="R56" s="24"/>
-      <c r="S56" s="24"/>
-      <c r="T56" s="24"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="19"/>
+      <c r="R56" s="19"/>
+      <c r="S56" s="19"/>
+      <c r="T56" s="19"/>
     </row>
     <row r="57" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H57" s="24" t="s">
+      <c r="H57" s="19" t="s">
         <v>9114</v>
       </c>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
-      <c r="K57" s="24"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="24"/>
-      <c r="O57" s="24"/>
-      <c r="P57" s="24"/>
-      <c r="Q57" s="24"/>
-      <c r="R57" s="24"/>
-      <c r="S57" s="24"/>
-      <c r="T57" s="24"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="19"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="19"/>
+      <c r="S57" s="19"/>
+      <c r="T57" s="19"/>
     </row>
     <row r="58" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="H58" s="24" t="s">
+      <c r="H58" s="19" t="s">
         <v>9117</v>
       </c>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="24"/>
-      <c r="N58" s="24"/>
-      <c r="O58" s="24"/>
-      <c r="P58" s="24"/>
-      <c r="Q58" s="24"/>
-      <c r="R58" s="24"/>
-      <c r="S58" s="24"/>
-      <c r="T58" s="24"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="19"/>
+      <c r="P58" s="19"/>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="19"/>
+      <c r="S58" s="19"/>
+      <c r="T58" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="H58:T58"/>
-    <mergeCell ref="H53:T53"/>
-    <mergeCell ref="H54:T54"/>
-    <mergeCell ref="H55:T55"/>
-    <mergeCell ref="H56:T56"/>
-    <mergeCell ref="H57:T57"/>
-    <mergeCell ref="H48:T48"/>
-    <mergeCell ref="H49:T49"/>
-    <mergeCell ref="G50:T50"/>
-    <mergeCell ref="H51:T51"/>
-    <mergeCell ref="H52:T52"/>
-    <mergeCell ref="H44:T44"/>
-    <mergeCell ref="H39:T39"/>
-    <mergeCell ref="H45:T45"/>
-    <mergeCell ref="H46:T46"/>
-    <mergeCell ref="H47:T47"/>
-    <mergeCell ref="H38:T38"/>
-    <mergeCell ref="G40:T40"/>
-    <mergeCell ref="H41:T41"/>
-    <mergeCell ref="H42:T42"/>
-    <mergeCell ref="H43:T43"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="G4:T4"/>
+    <mergeCell ref="G7:T7"/>
+    <mergeCell ref="G6:T6"/>
+    <mergeCell ref="G8:T8"/>
+    <mergeCell ref="G9:T9"/>
+    <mergeCell ref="H10:T10"/>
+    <mergeCell ref="H11:T11"/>
+    <mergeCell ref="H13:T13"/>
+    <mergeCell ref="H12:T12"/>
+    <mergeCell ref="H14:T14"/>
+    <mergeCell ref="H20:T20"/>
+    <mergeCell ref="H22:T22"/>
+    <mergeCell ref="G21:T21"/>
+    <mergeCell ref="H23:T23"/>
+    <mergeCell ref="H15:T15"/>
+    <mergeCell ref="G16:T16"/>
+    <mergeCell ref="H17:T17"/>
+    <mergeCell ref="H18:T18"/>
+    <mergeCell ref="H19:T19"/>
+    <mergeCell ref="H24:T24"/>
+    <mergeCell ref="H25:T25"/>
+    <mergeCell ref="H26:T26"/>
+    <mergeCell ref="H27:T27"/>
+    <mergeCell ref="H28:T28"/>
     <mergeCell ref="H35:T35"/>
     <mergeCell ref="H36:T36"/>
     <mergeCell ref="G34:T34"/>
@@ -29703,36 +29714,27 @@
     <mergeCell ref="H31:T31"/>
     <mergeCell ref="H32:T32"/>
     <mergeCell ref="H33:T33"/>
-    <mergeCell ref="H24:T24"/>
-    <mergeCell ref="H25:T25"/>
-    <mergeCell ref="H26:T26"/>
-    <mergeCell ref="H27:T27"/>
-    <mergeCell ref="H28:T28"/>
-    <mergeCell ref="H20:T20"/>
-    <mergeCell ref="H22:T22"/>
-    <mergeCell ref="G21:T21"/>
-    <mergeCell ref="H23:T23"/>
-    <mergeCell ref="H15:T15"/>
-    <mergeCell ref="G16:T16"/>
-    <mergeCell ref="H17:T17"/>
-    <mergeCell ref="H18:T18"/>
-    <mergeCell ref="H19:T19"/>
-    <mergeCell ref="H10:T10"/>
-    <mergeCell ref="H11:T11"/>
-    <mergeCell ref="H13:T13"/>
-    <mergeCell ref="H12:T12"/>
-    <mergeCell ref="H14:T14"/>
-    <mergeCell ref="G4:T4"/>
-    <mergeCell ref="G7:T7"/>
-    <mergeCell ref="G6:T6"/>
-    <mergeCell ref="G8:T8"/>
-    <mergeCell ref="G9:T9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="H38:T38"/>
+    <mergeCell ref="G40:T40"/>
+    <mergeCell ref="H41:T41"/>
+    <mergeCell ref="H42:T42"/>
+    <mergeCell ref="H43:T43"/>
+    <mergeCell ref="H44:T44"/>
+    <mergeCell ref="H39:T39"/>
+    <mergeCell ref="H45:T45"/>
+    <mergeCell ref="H46:T46"/>
+    <mergeCell ref="H47:T47"/>
+    <mergeCell ref="H48:T48"/>
+    <mergeCell ref="H49:T49"/>
+    <mergeCell ref="G50:T50"/>
+    <mergeCell ref="H51:T51"/>
+    <mergeCell ref="H52:T52"/>
+    <mergeCell ref="H58:T58"/>
+    <mergeCell ref="H53:T53"/>
+    <mergeCell ref="H54:T54"/>
+    <mergeCell ref="H55:T55"/>
+    <mergeCell ref="H56:T56"/>
+    <mergeCell ref="H57:T57"/>
   </mergeCells>
   <conditionalFormatting sqref="A28:A31">
     <cfRule type="expression" dxfId="4" priority="2">
@@ -34611,7 +34613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3361E218-E961-466F-899C-D4E612D4BCFC}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -35194,10 +35196,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC96714-4315-43B5-B8C3-4AD3885A6437}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35209,9 +35211,10 @@
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="73.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>258</v>
       </c>
@@ -35239,8 +35242,11 @@
       <c r="I1" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>733</v>
       </c>
@@ -35263,7 +35269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>735</v>
       </c>
@@ -35292,7 +35298,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>735</v>
       </c>
@@ -35321,7 +35327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>735</v>
       </c>
@@ -35347,7 +35353,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>735</v>
       </c>
@@ -35373,7 +35379,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>735</v>
       </c>
@@ -35399,7 +35405,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>733</v>
       </c>
@@ -35422,7 +35428,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>733</v>
       </c>
@@ -35445,7 +35451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>733</v>
       </c>

</xml_diff>